<commit_message>
adding ACTIVATE cases to library
</commit_message>
<xml_diff>
--- a/notebooks/output_conversion_scm.xlsx
+++ b/notebooks/output_conversion_scm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ftornow/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC453CD-B4B2-1744-8616-4AFE2451D33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EB1814-3FEF-D348-BE12-3CACBF8595E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36280" yWindow="-5620" windowWidth="34560" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="296">
   <si>
     <t>standard_name</t>
   </si>
@@ -982,6 +982,15 @@
   </si>
   <si>
     <t>assuming Nd = 60. cm-3 for condensate portion from convective scheme</t>
+  </si>
+  <si>
+    <t>cloud_area_fraction</t>
+  </si>
+  <si>
+    <t>clt</t>
+  </si>
+  <si>
+    <t>diagnosed cloud cover</t>
   </si>
 </sst>
 </file>
@@ -1426,10 +1435,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1060"/>
+  <dimension ref="A1:Z1061"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2182,10 +2191,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>61</v>
+        <v>293</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>62</v>
+        <v>294</v>
       </c>
       <c r="C21" s="18">
         <v>1</v>
@@ -2193,8 +2202,8 @@
       <c r="D21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>63</v>
+      <c r="E21" s="11" t="s">
+        <v>295</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -2220,19 +2229,19 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="19">
+        <v>61</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="18">
         <v>1</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>66</v>
+      <c r="E22" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2258,19 +2267,19 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="18">
+        <v>64</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="19">
         <v>1</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2296,10 +2305,10 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="18">
         <v>1</v>
@@ -2308,7 +2317,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2334,19 +2343,19 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>289</v>
+        <v>70</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>291</v>
+        <v>71</v>
+      </c>
+      <c r="C25" s="18">
+        <v>1</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>292</v>
+        <v>72</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -2371,20 +2380,20 @@
       <c r="Z25" s="17"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="14" t="s">
-        <v>73</v>
+      <c r="A26" s="12" t="s">
+        <v>289</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>75</v>
+        <v>290</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>291</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>76</v>
+        <v>292</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -2409,11 +2418,11 @@
       <c r="Z26" s="17"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="12" t="s">
-        <v>77</v>
+      <c r="A27" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>75</v>
@@ -2422,7 +2431,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -2447,20 +2456,20 @@
       <c r="Z27" s="17"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="14" t="s">
-        <v>80</v>
+      <c r="A28" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>7</v>
+      <c r="E28" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
@@ -2486,10 +2495,10 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>37</v>
@@ -2524,10 +2533,10 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>37</v>
@@ -2561,20 +2570,20 @@
       <c r="Z30" s="17"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>88</v>
+      <c r="A31" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>89</v>
+      <c r="E31" s="16" t="s">
+        <v>7</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>
@@ -2599,58 +2608,58 @@
       <c r="Z31" s="17"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
+      <c r="A32" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -2676,10 +2685,10 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>27</v>
@@ -2713,20 +2722,20 @@
       <c r="Z34" s="7"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="20" t="s">
-        <v>97</v>
+      <c r="A35" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -2751,20 +2760,20 @@
       <c r="Z35" s="7"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>101</v>
+      <c r="A36" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -2790,13 +2799,13 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>15</v>
@@ -2828,19 +2837,19 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" s="8">
-        <v>1</v>
+        <v>104</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
@@ -2866,10 +2875,10 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C39" s="8">
         <v>1</v>
@@ -2878,7 +2887,7 @@
         <v>15</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -2904,19 +2913,19 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>24</v>
+        <v>110</v>
+      </c>
+      <c r="C40" s="8">
+        <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -2942,19 +2951,19 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>105</v>
+        <v>113</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -2980,10 +2989,10 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>105</v>
@@ -2992,7 +3001,7 @@
         <v>15</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
@@ -3018,10 +3027,10 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>105</v>
@@ -3030,7 +3039,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -3056,19 +3065,19 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" s="8">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -3094,10 +3103,10 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C45" s="8">
         <v>1</v>
@@ -3106,7 +3115,7 @@
         <v>15</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -3132,10 +3141,10 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C46" s="8">
         <v>1</v>
@@ -3144,7 +3153,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
@@ -3170,19 +3179,19 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>75</v>
+        <v>128</v>
+      </c>
+      <c r="C47" s="8">
+        <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
@@ -3208,10 +3217,10 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>75</v>
@@ -3220,7 +3229,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -3246,19 +3255,19 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
@@ -3284,19 +3293,19 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>140</v>
+        <v>7</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -3322,19 +3331,19 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
@@ -3360,10 +3369,10 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>136</v>
@@ -3398,10 +3407,10 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>136</v>
@@ -3436,13 +3445,13 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>15</v>
@@ -3474,10 +3483,10 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>150</v>
@@ -3486,7 +3495,7 @@
         <v>15</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
@@ -3512,19 +3521,19 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
@@ -3550,10 +3559,10 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>156</v>
@@ -3562,7 +3571,7 @@
         <v>15</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
@@ -3588,19 +3597,19 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>75</v>
+        <v>156</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
@@ -3626,10 +3635,10 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>75</v>
@@ -3664,13 +3673,13 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>15</v>
@@ -3702,10 +3711,10 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>37</v>
@@ -3740,19 +3749,19 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>170</v>
+        <v>37</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>171</v>
+        <v>7</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -3778,10 +3787,10 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>170</v>
@@ -3790,7 +3799,7 @@
         <v>15</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -3816,10 +3825,10 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>170</v>
@@ -3828,7 +3837,7 @@
         <v>15</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -3854,19 +3863,19 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -3890,12 +3899,12 @@
       <c r="Y65" s="7"/>
       <c r="Z65" s="7"/>
     </row>
-    <row r="66" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>180</v>
@@ -3904,7 +3913,7 @@
         <v>15</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -3930,19 +3939,19 @@
     </row>
     <row r="67" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -3968,10 +3977,10 @@
     </row>
     <row r="68" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>185</v>
@@ -3980,7 +3989,7 @@
         <v>15</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -4006,10 +4015,10 @@
     </row>
     <row r="69" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>185</v>
@@ -4018,7 +4027,7 @@
         <v>15</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -4042,21 +4051,21 @@
       <c r="Y69" s="7"/>
       <c r="Z69" s="7"/>
     </row>
-    <row r="70" spans="1:26" ht="56" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -4082,10 +4091,10 @@
     </row>
     <row r="71" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>195</v>
@@ -4094,7 +4103,7 @@
         <v>15</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -4118,12 +4127,12 @@
       <c r="Y71" s="7"/>
       <c r="Z71" s="7"/>
     </row>
-    <row r="72" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>195</v>
@@ -4132,7 +4141,7 @@
         <v>15</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
@@ -4158,10 +4167,10 @@
     </row>
     <row r="73" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>195</v>
@@ -4170,7 +4179,7 @@
         <v>15</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
@@ -4194,12 +4203,12 @@
       <c r="Y73" s="7"/>
       <c r="Z73" s="7"/>
     </row>
-    <row r="74" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>195</v>
@@ -4208,7 +4217,7 @@
         <v>15</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -4234,10 +4243,10 @@
     </row>
     <row r="75" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>195</v>
@@ -4246,7 +4255,7 @@
         <v>15</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -4270,50 +4279,50 @@
       <c r="Y75" s="7"/>
       <c r="Z75" s="7"/>
     </row>
-    <row r="76" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A76" s="21" t="s">
+    <row r="76" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A76" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="7"/>
+      <c r="P76" s="7"/>
+      <c r="Q76" s="7"/>
+      <c r="R76" s="7"/>
+      <c r="S76" s="7"/>
+      <c r="T76" s="7"/>
+      <c r="U76" s="7"/>
+      <c r="V76" s="7"/>
+      <c r="W76" s="7"/>
+      <c r="X76" s="7"/>
+      <c r="Y76" s="7"/>
+      <c r="Z76" s="7"/>
+    </row>
+    <row r="77" spans="1:26" ht="56" x14ac:dyDescent="0.15">
+      <c r="A77" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="B76" s="22" t="s">
+      <c r="B77" s="22" t="s">
         <v>213</v>
-      </c>
-      <c r="C76" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
-      <c r="I76" s="25"/>
-      <c r="J76" s="25"/>
-      <c r="K76" s="25"/>
-      <c r="L76" s="25"/>
-      <c r="M76" s="25"/>
-      <c r="N76" s="25"/>
-      <c r="O76" s="25"/>
-      <c r="P76" s="25"/>
-      <c r="Q76" s="25"/>
-      <c r="R76" s="25"/>
-      <c r="S76" s="25"/>
-      <c r="T76" s="25"/>
-      <c r="U76" s="25"/>
-      <c r="V76" s="25"/>
-      <c r="W76" s="25"/>
-      <c r="X76" s="25"/>
-      <c r="Y76" s="25"/>
-      <c r="Z76" s="25"/>
-    </row>
-    <row r="77" spans="1:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="A77" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>216</v>
       </c>
       <c r="C77" s="23" t="s">
         <v>105</v>
@@ -4322,7 +4331,7 @@
         <v>15</v>
       </c>
       <c r="E77" s="24" t="s">
-        <v>7</v>
+        <v>214</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>
@@ -4346,12 +4355,12 @@
       <c r="Y77" s="25"/>
       <c r="Z77" s="25"/>
     </row>
-    <row r="78" spans="1:26" ht="42" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="21" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C78" s="23" t="s">
         <v>105</v>
@@ -4360,7 +4369,7 @@
         <v>15</v>
       </c>
       <c r="E78" s="24" t="s">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="F78" s="25"/>
       <c r="G78" s="25"/>
@@ -4384,12 +4393,12 @@
       <c r="Y78" s="25"/>
       <c r="Z78" s="25"/>
     </row>
-    <row r="79" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A79" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C79" s="23" t="s">
         <v>105</v>
@@ -4398,7 +4407,7 @@
         <v>15</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>7</v>
+        <v>219</v>
       </c>
       <c r="F79" s="25"/>
       <c r="G79" s="25"/>
@@ -4424,10 +4433,10 @@
     </row>
     <row r="80" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C80" s="23" t="s">
         <v>105</v>
@@ -4462,10 +4471,10 @@
     </row>
     <row r="81" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C81" s="23" t="s">
         <v>105</v>
@@ -4500,10 +4509,10 @@
     </row>
     <row r="82" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C82" s="23" t="s">
         <v>105</v>
@@ -4538,10 +4547,10 @@
     </row>
     <row r="83" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C83" s="23" t="s">
         <v>105</v>
@@ -4574,20 +4583,22 @@
       <c r="Y83" s="25"/>
       <c r="Z83" s="25"/>
     </row>
-    <row r="84" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A84" s="21" t="s">
-        <v>286</v>
+        <v>228</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>287</v>
+        <v>229</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>185</v>
+        <v>105</v>
       </c>
       <c r="D84" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E84" s="24"/>
+      <c r="E84" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
@@ -4610,22 +4621,20 @@
       <c r="Y84" s="25"/>
       <c r="Z84" s="25"/>
     </row>
-    <row r="85" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="21" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="C85" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" s="23" t="s">
         <v>185</v>
       </c>
       <c r="D85" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E85" s="24" t="s">
-        <v>232</v>
-      </c>
+      <c r="E85" s="24"/>
       <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
@@ -4648,12 +4657,12 @@
       <c r="Y85" s="25"/>
       <c r="Z85" s="25"/>
     </row>
-    <row r="86" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A86" s="21" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C86" s="22" t="s">
         <v>185</v>
@@ -4662,7 +4671,7 @@
         <v>15</v>
       </c>
       <c r="E86" s="24" t="s">
-        <v>7</v>
+        <v>232</v>
       </c>
       <c r="F86" s="25"/>
       <c r="G86" s="25"/>
@@ -4686,12 +4695,12 @@
       <c r="Y86" s="25"/>
       <c r="Z86" s="25"/>
     </row>
-    <row r="87" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C87" s="22" t="s">
         <v>185</v>
@@ -4700,7 +4709,7 @@
         <v>15</v>
       </c>
       <c r="E87" s="24" t="s">
-        <v>237</v>
+        <v>7</v>
       </c>
       <c r="F87" s="25"/>
       <c r="G87" s="25"/>
@@ -4724,12 +4733,12 @@
       <c r="Y87" s="25"/>
       <c r="Z87" s="25"/>
     </row>
-    <row r="88" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A88" s="21" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C88" s="22" t="s">
         <v>185</v>
@@ -4738,7 +4747,7 @@
         <v>15</v>
       </c>
       <c r="E88" s="24" t="s">
-        <v>7</v>
+        <v>237</v>
       </c>
       <c r="F88" s="25"/>
       <c r="G88" s="25"/>
@@ -4762,12 +4771,12 @@
       <c r="Y88" s="25"/>
       <c r="Z88" s="25"/>
     </row>
-    <row r="89" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A89" s="21" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>285</v>
+        <v>239</v>
       </c>
       <c r="C89" s="22" t="s">
         <v>185</v>
@@ -4775,7 +4784,9 @@
       <c r="D89" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E89" s="24"/>
+      <c r="E89" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="F89" s="25"/>
       <c r="G89" s="25"/>
       <c r="H89" s="25"/>
@@ -4798,22 +4809,20 @@
       <c r="Y89" s="25"/>
       <c r="Z89" s="25"/>
     </row>
-    <row r="90" spans="1:26" ht="28" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="21" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>241</v>
+        <v>285</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="D90" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E90" s="24" t="s">
-        <v>242</v>
-      </c>
+      <c r="E90" s="24"/>
       <c r="F90" s="25"/>
       <c r="G90" s="25"/>
       <c r="H90" s="25"/>
@@ -4836,12 +4845,12 @@
       <c r="Y90" s="25"/>
       <c r="Z90" s="25"/>
     </row>
-    <row r="91" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="21" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>30</v>
@@ -4850,7 +4859,7 @@
         <v>15</v>
       </c>
       <c r="E91" s="24" t="s">
-        <v>7</v>
+        <v>242</v>
       </c>
       <c r="F91" s="25"/>
       <c r="G91" s="25"/>
@@ -4876,10 +4885,10 @@
     </row>
     <row r="92" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A92" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C92" s="22" t="s">
         <v>30</v>
@@ -4914,10 +4923,10 @@
     </row>
     <row r="93" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A93" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C93" s="22" t="s">
         <v>30</v>
@@ -4952,19 +4961,19 @@
     </row>
     <row r="94" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="C94" s="23">
-        <v>1</v>
+        <v>248</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="D94" s="22" t="s">
         <v>15</v>
       </c>
       <c r="E94" s="24" t="s">
-        <v>251</v>
+        <v>7</v>
       </c>
       <c r="F94" s="25"/>
       <c r="G94" s="25"/>
@@ -4990,10 +4999,10 @@
     </row>
     <row r="95" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="21" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C95" s="23">
         <v>1</v>
@@ -5002,7 +5011,7 @@
         <v>15</v>
       </c>
       <c r="E95" s="24" t="s">
-        <v>7</v>
+        <v>251</v>
       </c>
       <c r="F95" s="25"/>
       <c r="G95" s="25"/>
@@ -5028,10 +5037,10 @@
     </row>
     <row r="96" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A96" s="21" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C96" s="23">
         <v>1</v>
@@ -5040,7 +5049,7 @@
         <v>15</v>
       </c>
       <c r="E96" s="24" t="s">
-        <v>256</v>
+        <v>7</v>
       </c>
       <c r="F96" s="25"/>
       <c r="G96" s="25"/>
@@ -5066,10 +5075,10 @@
     </row>
     <row r="97" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="21" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C97" s="23">
         <v>1</v>
@@ -5078,7 +5087,7 @@
         <v>15</v>
       </c>
       <c r="E97" s="24" t="s">
-        <v>7</v>
+        <v>256</v>
       </c>
       <c r="F97" s="25"/>
       <c r="G97" s="25"/>
@@ -5104,10 +5113,10 @@
     </row>
     <row r="98" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C98" s="23">
         <v>1</v>
@@ -5142,10 +5151,10 @@
     </row>
     <row r="99" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A99" s="21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C99" s="23">
         <v>1</v>
@@ -5180,10 +5189,10 @@
     </row>
     <row r="100" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A100" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C100" s="23">
         <v>1</v>
@@ -5218,10 +5227,10 @@
     </row>
     <row r="101" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C101" s="23">
         <v>1</v>
@@ -5256,19 +5265,19 @@
     </row>
     <row r="102" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A102" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="C102" s="23" t="s">
-        <v>27</v>
+        <v>266</v>
+      </c>
+      <c r="C102" s="23">
+        <v>1</v>
       </c>
       <c r="D102" s="22" t="s">
         <v>15</v>
       </c>
       <c r="E102" s="24" t="s">
-        <v>269</v>
+        <v>7</v>
       </c>
       <c r="F102" s="25"/>
       <c r="G102" s="25"/>
@@ -5294,10 +5303,10 @@
     </row>
     <row r="103" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B103" s="22" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C103" s="23" t="s">
         <v>27</v>
@@ -5306,7 +5315,7 @@
         <v>15</v>
       </c>
       <c r="E103" s="24" t="s">
-        <v>7</v>
+        <v>269</v>
       </c>
       <c r="F103" s="25"/>
       <c r="G103" s="25"/>
@@ -5332,10 +5341,10 @@
     </row>
     <row r="104" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C104" s="23" t="s">
         <v>27</v>
@@ -5344,7 +5353,7 @@
         <v>15</v>
       </c>
       <c r="E104" s="24" t="s">
-        <v>274</v>
+        <v>7</v>
       </c>
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
@@ -5370,10 +5379,10 @@
     </row>
     <row r="105" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C105" s="23" t="s">
         <v>27</v>
@@ -5382,7 +5391,7 @@
         <v>15</v>
       </c>
       <c r="E105" s="24" t="s">
-        <v>7</v>
+        <v>274</v>
       </c>
       <c r="F105" s="25"/>
       <c r="G105" s="25"/>
@@ -5408,10 +5417,10 @@
     </row>
     <row r="106" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A106" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C106" s="23" t="s">
         <v>27</v>
@@ -5446,10 +5455,10 @@
     </row>
     <row r="107" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A107" s="21" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C107" s="23" t="s">
         <v>27</v>
@@ -5484,10 +5493,10 @@
     </row>
     <row r="108" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A108" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C108" s="23" t="s">
         <v>27</v>
@@ -5522,10 +5531,10 @@
     </row>
     <row r="109" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A109" s="21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C109" s="23" t="s">
         <v>27</v>
@@ -5558,8 +5567,43 @@
       <c r="Y109" s="25"/>
       <c r="Z109" s="25"/>
     </row>
-    <row r="112" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="E112" s="26"/>
+    <row r="110" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+      <c r="A110" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B110" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110" s="25"/>
+      <c r="G110" s="25"/>
+      <c r="H110" s="25"/>
+      <c r="I110" s="25"/>
+      <c r="J110" s="25"/>
+      <c r="K110" s="25"/>
+      <c r="L110" s="25"/>
+      <c r="M110" s="25"/>
+      <c r="N110" s="25"/>
+      <c r="O110" s="25"/>
+      <c r="P110" s="25"/>
+      <c r="Q110" s="25"/>
+      <c r="R110" s="25"/>
+      <c r="S110" s="25"/>
+      <c r="T110" s="25"/>
+      <c r="U110" s="25"/>
+      <c r="V110" s="25"/>
+      <c r="W110" s="25"/>
+      <c r="X110" s="25"/>
+      <c r="Y110" s="25"/>
+      <c r="Z110" s="25"/>
     </row>
     <row r="113" spans="5:5" ht="13" x14ac:dyDescent="0.15">
       <c r="E113" s="26"/>
@@ -8404,6 +8448,9 @@
     </row>
     <row r="1060" spans="5:5" ht="13" x14ac:dyDescent="0.15">
       <c r="E1060" s="26"/>
+    </row>
+    <row r="1061" spans="5:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="E1061" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>